<commit_message>
friday work, pretty much finished with interface and login
</commit_message>
<xml_diff>
--- a/zdoc/Software Project Requirements.xlsx
+++ b/zdoc/Software Project Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephsoriano/Desktop/School/2019 Spring/CSE 3310/Project/Superchat/doc/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephsoriano/Desktop/School/2019 Spring/CSE 3310/Project/Superchat/zdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA9F500-A057-4246-BF8C-419E14AA0542}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08F0577-E88C-F949-A643-A6520C15D198}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{8E689F70-54D6-C242-BE1D-4E59EC62B863}"/>
   </bookViews>
@@ -607,7 +607,23 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -708,6 +724,22 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -741,39 +773,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -868,13 +868,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25410F8A-371E-0247-A9B9-8551A391583F}" name="Table2" displayName="Table2" ref="A1:G34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="A1:G34" xr:uid="{F05985FA-B9EA-F449-A6C7-F9E9AA7DABD9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D07A80DD-AC43-DA42-ABB9-6917EE1B8195}" name="Identifier" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{A59C9F51-1B73-4D44-BB3C-ADD4E5CA8D26}" name="Requirement" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{894E95CF-9AE1-6D4F-86DF-05B7DDA90BBC}" name="Functional/ Non Functional" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4D635445-D29B-F04D-BE43-AB8F3A7704C4}" name="Source" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{E60B3A75-156D-F645-AF89-32B86DF5C0B8}" name="Client/Server/Both" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{44E3CF39-3CA5-D746-95A7-BE0099C74661}" name="Notes" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{40A62C7A-29AA-D747-A2D7-F498512DA341}" name="Function" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D07A80DD-AC43-DA42-ABB9-6917EE1B8195}" name="Identifier" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A59C9F51-1B73-4D44-BB3C-ADD4E5CA8D26}" name="Requirement" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{894E95CF-9AE1-6D4F-86DF-05B7DDA90BBC}" name="Functional/ Non Functional" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{4D635445-D29B-F04D-BE43-AB8F3A7704C4}" name="Source" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{E60B3A75-156D-F645-AF89-32B86DF5C0B8}" name="Client/Server/Both" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{44E3CF39-3CA5-D746-95A7-BE0099C74661}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{40A62C7A-29AA-D747-A2D7-F498512DA341}" name="Function" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3870C74C-FCB0-9F43-AAF6-BFB2D9C0C9DB}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G33" sqref="A1:G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="72" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>